<commit_message>
Ajustes etapa 1, desarrollo etapa 2 y 3.
Se adjuntan notas en el archivo excel, igualmente estructuras con
demasiadas variaciones tienen su captura de pantalla y su HTML.
</commit_message>
<xml_diff>
--- a/Listado páginas.xlsx
+++ b/Listado páginas.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="22515" windowHeight="8265"/>
+    <workbookView xWindow="240" yWindow="40" windowWidth="32820" windowHeight="17580"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
   <si>
     <t>Header y footer.</t>
   </si>
@@ -223,13 +228,64 @@
   </si>
   <si>
     <t>Resultado suscripción.</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Revision Coctel</t>
+  </si>
+  <si>
+    <t>Revision Carvajal</t>
+  </si>
+  <si>
+    <t>No se tiene acceso, favor poner boton</t>
+  </si>
+  <si>
+    <t>Ajustes Realizados</t>
+  </si>
+  <si>
+    <t>OK pendiente ajuste estructura DIVS tanto del buscador como del contenido</t>
+  </si>
+  <si>
+    <t>OK pendiente resvisar un poco estructura de textos</t>
+  </si>
+  <si>
+    <t>OK pendiente estructura de textos</t>
+  </si>
+  <si>
+    <t>Esperando ajuste de orden en elementos</t>
+  </si>
+  <si>
+    <t>OK - Sky Scraper OK -  Falta texto por confirmar estructura</t>
+  </si>
+  <si>
+    <t>Revisar texto que esta suelto al interior de los divs</t>
+  </si>
+  <si>
+    <t>OK funciona igual que Home área temática</t>
+  </si>
+  <si>
+    <t>OK funciona con el general.css ya generado</t>
+  </si>
+  <si>
+    <t>OK ajustar botones por primary y colocar los a en los teléfonos</t>
+  </si>
+  <si>
+    <t>OK se ajusta con el CSS de Administración guía de proveedores - home.</t>
+  </si>
+  <si>
+    <t>OK pendiente ajuste textos superior</t>
+  </si>
+  <si>
+    <t>No hay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +299,21 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -269,31 +340,107 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="42">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -584,210 +731,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" customWidth="1"/>
-    <col min="2" max="2" width="133.42578125" customWidth="1"/>
+    <col min="1" max="1" width="51.5" customWidth="1"/>
+    <col min="2" max="2" width="133.5" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>67</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>68</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -795,7 +1048,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -803,7 +1056,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -814,7 +1067,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -825,7 +1078,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -836,12 +1089,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:6">
+      <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -852,7 +1110,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -863,7 +1121,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -874,22 +1132,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C36" t="s">
@@ -903,6 +1161,12 @@
     <hyperlink ref="B35" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -912,9 +1176,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -924,8 +1193,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega en contenido editorial otro link
</commit_message>
<xml_diff>
--- a/Listado páginas.xlsx
+++ b/Listado páginas.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="40" windowWidth="32820" windowHeight="17580"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>Header y footer.</t>
   </si>
@@ -140,9 +140,6 @@
     <t>inovom.pruebab2b.com/catalogos/</t>
   </si>
   <si>
-    <t>http://inovom.pruebab2b.com/temas/+113492,     http://inovom.pruebab2b.com/temas/+103286,   http://inovom.pruebab2b.com/temas/+3084014</t>
-  </si>
-  <si>
     <t>inovom.pruebab2b.com/blogs/</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>No hay</t>
+  </si>
+  <si>
+    <t>http://inovom.pruebab2b.com/temas/+113492,     http://inovom.pruebab2b.com/temas/+103286,   http://inovom.pruebab2b.com/temas/+3084014, http://inovom.pruebab2b.com/temas/+112326</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -394,6 +394,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -441,6 +444,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -733,20 +741,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5" customWidth="1"/>
-    <col min="2" max="2" width="133.5" customWidth="1"/>
-    <col min="4" max="4" width="60.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="133.42578125" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -755,16 +763,16 @@
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -772,16 +780,16 @@
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -789,10 +797,10 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -800,16 +808,16 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -817,46 +825,46 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
+        <v>66</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -866,84 +874,84 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -953,84 +961,84 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1040,56 +1048,53 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
       <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1099,59 +1104,47 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +1169,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1193,7 +1186,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Últimos ajustes para revision
Adjuntamos los temas hablados como las modales, el encabezado, el
footer, y de mas notas de la ultima reunion sostenida con Renzo.
</commit_message>
<xml_diff>
--- a/Listado páginas.xlsx
+++ b/Listado páginas.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="36240" windowHeight="16820"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="86">
   <si>
     <t>Header y footer.</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Ajustes Realizados</t>
   </si>
   <si>
-    <t>Esperando ajuste de orden en elementos</t>
-  </si>
-  <si>
     <t>Revisar texto que esta suelto al interior de los divs</t>
   </si>
   <si>
@@ -242,21 +239,12 @@
     <t>OK - colocar los link en los teléfonos</t>
   </si>
   <si>
-    <t>Galeria</t>
-  </si>
-  <si>
     <t xml:space="preserve">OK </t>
   </si>
   <si>
     <t>Pendiente</t>
   </si>
   <si>
-    <t>Pie ajustar centrado interior</t>
-  </si>
-  <si>
-    <t>OK  Header</t>
-  </si>
-  <si>
     <t>Revisar informacion del evento</t>
   </si>
   <si>
@@ -282,6 +270,15 @@
   </si>
   <si>
     <t>http://www.pruebab2b.com/copyright</t>
+  </si>
+  <si>
+    <t>Pie ajustar centrado interior - OK</t>
+  </si>
+  <si>
+    <t>Galeria - OK,  Modal Galería - OK</t>
+  </si>
+  <si>
+    <t>Se realiza revision del articulo destacado -Carvajal: revisar estructura de #articulo-destacado, pues hay elementos dentro de un col-sx-6 y unos textos estan fuera.</t>
   </si>
 </sst>
 </file>
@@ -343,9 +340,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="72">
+  <cellStyleXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -434,7 +433,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="72">
+  <cellStyles count="74">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="3" builtinId="9" hidden="1"/>
@@ -506,6 +505,8 @@
     <cellStyle name="Hipervínculo visitado" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -807,20 +808,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" customWidth="1"/>
-    <col min="2" max="2" width="102.42578125" customWidth="1"/>
+    <col min="1" max="1" width="51.5" customWidth="1"/>
+    <col min="2" max="2" width="102.5" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" customWidth="1"/>
-    <col min="6" max="6" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -838,7 +839,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -848,14 +849,11 @@
       <c r="D2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E2" t="s">
-        <v>77</v>
-      </c>
       <c r="F2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -869,10 +867,10 @@
         <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -886,10 +884,10 @@
         <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -903,27 +901,24 @@
         <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28">
       <c r="A6" t="s">
         <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" t="s">
-        <v>63</v>
-      </c>
       <c r="F6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -937,10 +932,10 @@
         <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -948,10 +943,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -961,7 +956,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="42">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -974,11 +969,11 @@
       <c r="E10" t="s">
         <v>63</v>
       </c>
-      <c r="F10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -986,16 +981,16 @@
         <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
         <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -1003,10 +998,10 @@
         <v>42</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1020,10 +1015,10 @@
         <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1034,10 +1029,10 @@
         <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1051,10 +1046,10 @@
         <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1065,10 +1060,10 @@
         <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1078,7 +1073,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1092,10 +1087,10 @@
         <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1103,10 +1098,10 @@
         <v>49</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1120,10 +1115,10 @@
         <v>63</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1137,10 +1132,10 @@
         <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1148,16 +1143,16 @@
         <v>52</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
         <v>63</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1171,10 +1166,10 @@
         <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1185,10 +1180,10 @@
         <v>63</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1198,7 +1193,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="42">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1206,10 +1201,10 @@
         <v>55</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1223,10 +1218,10 @@
         <v>63</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1238,7 +1233,7 @@
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1249,10 +1244,10 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1264,7 +1259,7 @@
       </c>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1274,51 +1269,51 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
         <v>57</v>
       </c>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D36" s="5"/>
     </row>
@@ -1347,7 +1342,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1364,7 +1359,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Actualización pendientes y link
</commit_message>
<xml_diff>
--- a/Listado páginas.xlsx
+++ b/Listado páginas.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="36240" windowHeight="16820"/>
+    <workbookView xWindow="45" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="85">
   <si>
     <t>Header y footer.</t>
   </si>
@@ -191,9 +191,6 @@
     <t>http://prueba.carvajalmediosb2b.com/guia-de-proveedores</t>
   </si>
   <si>
-    <t>inovom.pruebab2b.com/guia-de-proveedores/empresas/Dormer-Tools-SA+7803?showroom=99379</t>
-  </si>
-  <si>
     <t>PENDIENTE</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>Pendiente estructura header</t>
+  </si>
+  <si>
+    <t>http://www.pruebab2b.com/guia-de-proveedores/empresas/+513916,  http://www.pruebab2b.com/guia-de-proveedores/empresas/+10840</t>
   </si>
 </sst>
 </file>
@@ -825,20 +825,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5" customWidth="1"/>
-    <col min="2" max="2" width="95.5" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
-    <col min="6" max="6" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -847,16 +847,16 @@
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -864,13 +864,13 @@
         <v>35</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -878,16 +878,16 @@
         <v>36</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -895,16 +895,16 @@
         <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -912,30 +912,30 @@
         <v>38</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="28">
-      <c r="A6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -943,16 +943,16 @@
         <v>39</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -960,10 +960,10 @@
         <v>40</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -973,7 +973,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="42">
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -981,16 +981,16 @@
         <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -998,27 +998,27 @@
         <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1026,16 +1026,16 @@
         <v>43</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1043,13 +1043,13 @@
         <v>44</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1057,16 +1057,16 @@
         <v>45</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1074,13 +1074,13 @@
         <v>47</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1090,7 +1090,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1098,16 +1098,16 @@
         <v>48</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1115,10 +1115,10 @@
         <v>49</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1126,16 +1126,16 @@
         <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1143,16 +1143,16 @@
         <v>51</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1160,16 +1160,16 @@
         <v>52</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1177,16 +1177,16 @@
         <v>53</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1194,13 +1194,13 @@
         <v>54</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" ht="42">
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1218,65 +1218,62 @@
         <v>55</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
-      <c r="B28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
+      <c r="B28" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1286,60 +1283,60 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" ht="42">
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="42">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="42">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1367,7 +1364,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1384,7 +1381,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Se quita pendiente - quienes somos
Se quita pendiente - quienes somos
</commit_message>
<xml_diff>
--- a/Listado páginas.xlsx
+++ b/Listado páginas.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10880" yWindow="2620" windowWidth="33320" windowHeight="18220"/>
+    <workbookView xWindow="10875" yWindow="2625" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
   <si>
     <t>Header y footer.</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t>http://prueba.carvajalmediosb2b.com/guia-de-proveedores</t>
-  </si>
-  <si>
-    <t>PENDIENTE</t>
   </si>
   <si>
     <t>inovom.pruebab2b.com/temas</t>
@@ -495,6 +492,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -787,20 +789,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5" customWidth="1"/>
-    <col min="2" max="2" width="95.5" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="95.42578125" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
-    <col min="6" max="6" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -809,16 +811,16 @@
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -826,16 +828,16 @@
         <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -843,16 +845,16 @@
         <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -860,16 +862,16 @@
         <v>36</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -877,33 +879,33 @@
         <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="28">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -911,16 +913,16 @@
         <v>38</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -928,16 +930,16 @@
         <v>39</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -947,7 +949,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -955,16 +957,16 @@
         <v>40</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -972,33 +974,33 @@
         <v>45</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1006,16 +1008,16 @@
         <v>42</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1023,16 +1025,16 @@
         <v>43</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1040,16 +1042,16 @@
         <v>44</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1057,16 +1059,16 @@
         <v>46</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1076,7 +1078,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1084,16 +1086,16 @@
         <v>47</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1101,16 +1103,16 @@
         <v>48</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1118,16 +1120,16 @@
         <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1135,16 +1137,16 @@
         <v>50</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1152,16 +1154,16 @@
         <v>51</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1169,16 +1171,16 @@
         <v>52</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1186,16 +1188,16 @@
         <v>53</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1205,7 +1207,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1213,67 +1215,67 @@
         <v>54</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="17" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1283,60 +1285,57 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" ht="42">
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="42">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="42">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1364,7 +1363,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1381,7 +1380,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>